<commit_message>
Some updates to CATS + default scenario
Fixed some issues with how fuel constraints from past years were propagated through model.  Template now will generate correctly.
</commit_message>
<xml_diff>
--- a/scenarios/BAUScenario/scenario_inputs_BAU.xlsx
+++ b/scenarios/BAUScenario/scenario_inputs_BAU.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://carb-my.sharepoint.com/personal/jeff_kessler_arb_ca_gov/Documents/Documents/GitHub/CATS/scenarios/BAUScenario/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="800" documentId="108_{45618FC2-8E48-4B2A-A13D-96D16367B1EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3A646AE0-5216-49EA-8CB1-A647AC58B1C0}"/>
+  <xr:revisionPtr revIDLastSave="892" documentId="108_{45618FC2-8E48-4B2A-A13D-96D16367B1EC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{81F74DCD-2D9E-405E-B08E-5E4CF72B7DE4}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21990" windowHeight="13410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21990" windowHeight="13410" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Energy Demand" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,9 @@
     <sheet name="Blend Requirements" sheetId="9" r:id="rId10"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Fuel Production'!$A$1:$U$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Fuel Production'!$A$1:$U$73</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="145">
   <si>
     <t>Year</t>
   </si>
@@ -462,12 +462,6 @@
     <t>Landfill CNG</t>
   </si>
   <si>
-    <t>HDV-H2 (0-CI)</t>
-  </si>
-  <si>
-    <t>LDV-H2 (0-CI)</t>
-  </si>
-  <si>
     <t>Dairy Gas for CNG</t>
   </si>
   <si>
@@ -475,6 +469,15 @@
   </si>
   <si>
     <t>NG for CNG</t>
+  </si>
+  <si>
+    <t>HDV Hydrogen (0-CI)</t>
+  </si>
+  <si>
+    <t>LDV Hydrogen (0-CI)</t>
+  </si>
+  <si>
+    <t>E85 w. CCS</t>
   </si>
 </sst>
 </file>
@@ -617,7 +620,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -657,6 +660,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -4534,10 +4538,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4593,7 +4597,19 @@
         <v>132</v>
       </c>
       <c r="C4">
-        <v>4528398004</v>
+        <v>5568655430</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2022</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <f>50*1000000*80</f>
+        <v>4000000000</v>
       </c>
     </row>
   </sheetData>
@@ -4603,11 +4619,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Sheet3" filterMode="1"/>
-  <dimension ref="A1:U56"/>
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:U73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="116" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="R47" sqref="R47"/>
+    <sheetView topLeftCell="A9" zoomScale="116" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4617,10 +4633,10 @@
     <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" hidden="1" customWidth="1"/>
-    <col min="9" max="11" width="15.7109375" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="48.85546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="48.85546875" customWidth="1"/>
     <col min="13" max="14" width="18.140625" customWidth="1"/>
     <col min="15" max="15" width="21.140625" customWidth="1"/>
     <col min="16" max="16" width="18.85546875" customWidth="1"/>
@@ -4697,7 +4713,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2022</v>
       </c>
@@ -4757,7 +4773,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2022</v>
       </c>
@@ -4814,7 +4830,7 @@
         <v>7.713073659853452E-9</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -4874,7 +4890,7 @@
         <v>7.9283279156425911E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -4982,7 +4998,7 @@
         <v>59</v>
       </c>
       <c r="R6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="S6" t="s">
         <v>109</v>
@@ -5040,7 +5056,7 @@
         <v>59</v>
       </c>
       <c r="R7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="S7" t="s">
         <v>109</v>
@@ -5050,7 +5066,7 @@
         <v>7.436602959767978E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2033</v>
       </c>
@@ -5101,7 +5117,7 @@
         <v>2.7777777777777781E-7</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2022</v>
       </c>
@@ -5152,7 +5168,7 @@
         <v>2.7777777777777781E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2022</v>
       </c>
@@ -5203,7 +5219,7 @@
         <v>2.7777777777777781E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2022</v>
       </c>
@@ -5266,7 +5282,7 @@
         <v>1.2268433321064899E-8</v>
       </c>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2022</v>
       </c>
@@ -5320,7 +5336,7 @@
         <v>8.3661005605287371E-9</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2022</v>
       </c>
@@ -5374,7 +5390,7 @@
         <v>7.436602959767978E-9</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2022</v>
       </c>
@@ -5432,7 +5448,7 @@
         <v>1.2268433321064899E-8</v>
       </c>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2022</v>
       </c>
@@ -5446,15 +5462,13 @@
         <v>33</v>
       </c>
       <c r="E15">
-        <f>E2</f>
-        <v>925.08936202114103</v>
+        <v>872</v>
       </c>
       <c r="F15" t="s">
         <v>35</v>
       </c>
       <c r="G15">
-        <f>G2</f>
-        <v>38878.476647424846</v>
+        <v>35283</v>
       </c>
       <c r="H15" t="s">
         <v>34</v>
@@ -5492,7 +5506,7 @@
         <v>8.3661005605287371E-9</v>
       </c>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -5506,15 +5520,13 @@
         <v>37</v>
       </c>
       <c r="E16">
-        <f>E3</f>
-        <v>1121.7752316226699</v>
+        <v>1069</v>
       </c>
       <c r="F16" t="s">
         <v>35</v>
       </c>
       <c r="G16">
-        <f>G3</f>
-        <v>37655.020185298134</v>
+        <v>34173</v>
       </c>
       <c r="H16" t="s">
         <v>34</v>
@@ -5596,7 +5608,7 @@
         <v>59</v>
       </c>
       <c r="R17" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="S17" t="s">
         <v>109</v>
@@ -5606,7 +5618,7 @@
         <v>7.436602959767978E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2022</v>
       </c>
@@ -5620,13 +5632,13 @@
         <v>40</v>
       </c>
       <c r="E18">
-        <v>41.977465970365564</v>
+        <v>51.2</v>
       </c>
       <c r="F18" t="s">
         <v>66</v>
       </c>
       <c r="G18">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H18" t="s">
         <v>81</v>
@@ -5657,7 +5669,7 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2022</v>
       </c>
@@ -5671,13 +5683,13 @@
         <v>40</v>
       </c>
       <c r="E19">
-        <v>46.342077721810462</v>
+        <v>56.5</v>
       </c>
       <c r="F19" t="s">
         <v>66</v>
       </c>
       <c r="G19">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H19" t="s">
         <v>81</v>
@@ -5708,7 +5720,7 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2022</v>
       </c>
@@ -5722,13 +5734,13 @@
         <v>50</v>
       </c>
       <c r="E20">
-        <v>41.977465970365564</v>
+        <v>51.2</v>
       </c>
       <c r="F20" t="s">
         <v>66</v>
       </c>
       <c r="G20">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H20" t="s">
         <v>81</v>
@@ -5759,7 +5771,7 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2033</v>
       </c>
@@ -5773,13 +5785,13 @@
         <v>136</v>
       </c>
       <c r="E21">
-        <v>41.977465970365564</v>
+        <v>51.2</v>
       </c>
       <c r="F21" t="s">
         <v>66</v>
       </c>
       <c r="G21">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H21" t="s">
         <v>81</v>
@@ -5810,7 +5822,7 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="22" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2022</v>
       </c>
@@ -5825,14 +5837,13 @@
       </c>
       <c r="E22">
         <f>E15</f>
-        <v>925.08936202114103</v>
+        <v>872</v>
       </c>
       <c r="F22" t="s">
         <v>35</v>
       </c>
       <c r="G22">
-        <f>G15</f>
-        <v>38878.476647424846</v>
+        <v>35283</v>
       </c>
       <c r="H22" t="s">
         <v>34</v>
@@ -5870,7 +5881,7 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="23" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2022</v>
       </c>
@@ -5885,14 +5896,13 @@
       </c>
       <c r="E23">
         <f>E16</f>
-        <v>1121.7752316226699</v>
+        <v>1069</v>
       </c>
       <c r="F23" t="s">
         <v>35</v>
       </c>
       <c r="G23">
-        <f>G16</f>
-        <v>37655.020185298134</v>
+        <v>34173</v>
       </c>
       <c r="H23" t="s">
         <v>34</v>
@@ -5930,7 +5940,7 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="24" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2022</v>
       </c>
@@ -5979,7 +5989,7 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="25" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2022</v>
       </c>
@@ -6031,7 +6041,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="26" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2022</v>
       </c>
@@ -6091,34 +6101,34 @@
         <v>1.2268433321064899E-8</v>
       </c>
     </row>
-    <row r="27" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <f>E26</f>
+        <v>0.95</v>
       </c>
       <c r="F27" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27">
+        <v>235</v>
+      </c>
+      <c r="H27" t="s">
+        <v>73</v>
+      </c>
+      <c r="I27">
         <v>35</v>
-      </c>
-      <c r="G27">
-        <f>ROUND(33.78*126.37,0)</f>
-        <v>4269</v>
-      </c>
-      <c r="H27" t="s">
-        <v>68</v>
-      </c>
-      <c r="I27">
-        <v>89.15</v>
       </c>
       <c r="J27" t="s">
         <v>69</v>
@@ -6126,26 +6136,33 @@
       <c r="K27">
         <v>1</v>
       </c>
+      <c r="L27" t="s">
+        <v>85</v>
+      </c>
+      <c r="M27" s="11"/>
       <c r="O27" t="s">
-        <v>82</v>
+        <v>126</v>
       </c>
       <c r="P27" t="s">
-        <v>61</v>
+        <v>60</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>88</v>
       </c>
       <c r="R27" t="s">
-        <v>101</v>
+        <v>47</v>
       </c>
       <c r="S27" t="s">
         <v>107</v>
       </c>
       <c r="T27">
-        <f>1/129.69/1000000</f>
-        <v>7.7106947335954979E-9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+        <f>1/81.51/1000000</f>
+        <v>1.2268433321064899E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="B28" t="s">
         <v>54</v>
@@ -6170,7 +6187,7 @@
         <v>68</v>
       </c>
       <c r="I28">
-        <v>87.89</v>
+        <v>89.15</v>
       </c>
       <c r="J28" t="s">
         <v>69</v>
@@ -6191,13 +6208,13 @@
         <v>107</v>
       </c>
       <c r="T28">
-        <f t="shared" ref="T28:T34" si="0">1/129.69/1000000</f>
+        <f>1/129.69/1000000</f>
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="29" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -6215,14 +6232,14 @@
         <v>35</v>
       </c>
       <c r="G29">
-        <f t="shared" ref="G29:G34" si="1">ROUND(33.78*126.37,0)</f>
+        <f>ROUND(33.78*126.37,0)</f>
         <v>4269</v>
       </c>
       <c r="H29" t="s">
         <v>68</v>
       </c>
       <c r="I29">
-        <v>86.64</v>
+        <v>87.89</v>
       </c>
       <c r="J29" t="s">
         <v>69</v>
@@ -6243,13 +6260,13 @@
         <v>107</v>
       </c>
       <c r="T29">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="T29:T35" si="0">1/129.69/1000000</f>
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B30" t="s">
         <v>54</v>
@@ -6267,14 +6284,14 @@
         <v>35</v>
       </c>
       <c r="G30">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="G30:G35" si="1">ROUND(33.78*126.37,0)</f>
         <v>4269</v>
       </c>
       <c r="H30" t="s">
         <v>68</v>
       </c>
       <c r="I30">
-        <v>85.38</v>
+        <v>86.64</v>
       </c>
       <c r="J30" t="s">
         <v>69</v>
@@ -6299,9 +6316,9 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="31" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="B31" t="s">
         <v>54</v>
@@ -6326,7 +6343,7 @@
         <v>68</v>
       </c>
       <c r="I31">
-        <v>84.13</v>
+        <v>85.38</v>
       </c>
       <c r="J31" t="s">
         <v>69</v>
@@ -6351,9 +6368,9 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="32" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="B32" t="s">
         <v>54</v>
@@ -6378,7 +6395,7 @@
         <v>68</v>
       </c>
       <c r="I32">
-        <v>82.87</v>
+        <v>84.13</v>
       </c>
       <c r="J32" t="s">
         <v>69</v>
@@ -6403,9 +6420,9 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>2029</v>
+        <v>2028</v>
       </c>
       <c r="B33" t="s">
         <v>54</v>
@@ -6430,7 +6447,7 @@
         <v>68</v>
       </c>
       <c r="I33">
-        <v>81.62</v>
+        <v>82.87</v>
       </c>
       <c r="J33" t="s">
         <v>69</v>
@@ -6455,9 +6472,9 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="B34" t="s">
         <v>54</v>
@@ -6482,7 +6499,7 @@
         <v>68</v>
       </c>
       <c r="I34">
-        <v>80.36</v>
+        <v>81.62</v>
       </c>
       <c r="J34" t="s">
         <v>69</v>
@@ -6507,135 +6524,136 @@
         <v>7.7106947335954979E-9</v>
       </c>
     </row>
-    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2022</v>
+        <v>2030</v>
       </c>
       <c r="B35" t="s">
-        <v>90</v>
+        <v>54</v>
       </c>
       <c r="C35" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="D35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E35">
-        <v>41.977465970365564</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="G35">
-        <v>1055</v>
+        <f t="shared" si="1"/>
+        <v>4269</v>
       </c>
       <c r="H35" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="I35">
-        <v>144.13</v>
+        <v>80.36</v>
       </c>
       <c r="J35" t="s">
         <v>69</v>
       </c>
       <c r="K35">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="O35" t="s">
         <v>82</v>
       </c>
       <c r="P35" t="s">
+        <v>61</v>
+      </c>
+      <c r="R35" t="s">
+        <v>101</v>
+      </c>
+      <c r="S35" t="s">
+        <v>107</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="0"/>
+        <v>7.7106947335954979E-9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2022</v>
+      </c>
+      <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" t="s">
+        <v>40</v>
+      </c>
+      <c r="E36">
+        <v>51.2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G36">
+        <v>865.1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36">
+        <v>144.13</v>
+      </c>
+      <c r="J36" t="s">
+        <v>69</v>
+      </c>
+      <c r="K36">
+        <v>2.5</v>
+      </c>
+      <c r="O36" t="s">
+        <v>82</v>
+      </c>
+      <c r="P36" t="s">
         <v>60</v>
       </c>
-      <c r="R35" t="s">
+      <c r="R36" t="s">
         <v>103</v>
       </c>
-      <c r="S35" t="s">
+      <c r="S36" t="s">
         <v>108</v>
       </c>
-      <c r="T35">
+      <c r="T36">
         <f>1/120/1000000</f>
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>2022</v>
-      </c>
-      <c r="B36" t="s">
-        <v>91</v>
-      </c>
-      <c r="C36" t="s">
-        <v>89</v>
-      </c>
-      <c r="D36" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36">
-        <v>46.342077721810462</v>
-      </c>
-      <c r="F36" t="s">
-        <v>66</v>
-      </c>
-      <c r="G36">
-        <v>1055</v>
-      </c>
-      <c r="H36" t="s">
-        <v>81</v>
-      </c>
-      <c r="I36">
-        <v>54</v>
-      </c>
-      <c r="J36" t="s">
-        <v>69</v>
-      </c>
-      <c r="K36">
-        <v>2.5</v>
-      </c>
-      <c r="O36" t="s">
-        <v>82</v>
-      </c>
-      <c r="P36" t="s">
-        <v>60</v>
-      </c>
-      <c r="R36" t="s">
-        <v>103</v>
-      </c>
-      <c r="S36" t="s">
-        <v>108</v>
-      </c>
-      <c r="T36">
-        <f t="shared" ref="T36:T38" si="2">1/120/1000000</f>
-        <v>8.3333333333333335E-9</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2022</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C37" t="s">
         <v>89</v>
       </c>
       <c r="D37" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E37">
-        <v>41.977465970365564</v>
+        <v>56.5</v>
       </c>
       <c r="F37" t="s">
         <v>66</v>
       </c>
       <c r="G37">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H37" t="s">
         <v>81</v>
       </c>
       <c r="I37">
-        <v>116</v>
+        <v>54</v>
       </c>
       <c r="J37" t="s">
         <v>69</v>
@@ -6656,13 +6674,13 @@
         <v>108</v>
       </c>
       <c r="T37">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="T37:T39" si="2">1/120/1000000</f>
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>2033</v>
+        <v>2022</v>
       </c>
       <c r="B38" t="s">
         <v>90</v>
@@ -6671,22 +6689,22 @@
         <v>89</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="E38">
-        <v>41.977465970365564</v>
+        <v>51.2</v>
       </c>
       <c r="F38" t="s">
         <v>66</v>
       </c>
       <c r="G38">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H38" t="s">
         <v>81</v>
       </c>
-      <c r="I38" s="20">
-        <v>-267</v>
+      <c r="I38">
+        <v>116</v>
       </c>
       <c r="J38" t="s">
         <v>69</v>
@@ -6711,122 +6729,118 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39">
+        <v>2033</v>
+      </c>
+      <c r="B39" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" t="s">
+        <v>89</v>
+      </c>
+      <c r="D39" t="s">
+        <v>136</v>
+      </c>
+      <c r="E39">
+        <v>51.2</v>
+      </c>
+      <c r="F39" t="s">
+        <v>66</v>
+      </c>
+      <c r="G39">
+        <v>865.1</v>
+      </c>
+      <c r="H39" t="s">
+        <v>81</v>
+      </c>
+      <c r="I39" s="20">
+        <v>-267</v>
+      </c>
+      <c r="J39" t="s">
+        <v>69</v>
+      </c>
+      <c r="K39">
+        <v>2.5</v>
+      </c>
+      <c r="O39" t="s">
+        <v>82</v>
+      </c>
+      <c r="P39" t="s">
+        <v>60</v>
+      </c>
+      <c r="R39" t="s">
+        <v>103</v>
+      </c>
+      <c r="S39" t="s">
+        <v>108</v>
+      </c>
+      <c r="T39">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40">
         <v>2022</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>114</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>119</v>
       </c>
-      <c r="E39">
+      <c r="E40">
         <v>1000</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F40" t="s">
         <v>123</v>
       </c>
-      <c r="G39">
+      <c r="G40">
         <v>1</v>
       </c>
-      <c r="H39" t="s">
+      <c r="H40" t="s">
         <v>122</v>
       </c>
-      <c r="I39">
+      <c r="I40">
         <f>-1000000</f>
         <v>-1000000</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J40" t="s">
         <v>70</v>
       </c>
-      <c r="K39">
+      <c r="K40">
         <v>1</v>
       </c>
-      <c r="L39" t="s">
+      <c r="L40" t="s">
         <v>125</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O40" t="s">
         <v>114</v>
       </c>
-      <c r="P39" t="s">
+      <c r="P40" t="s">
         <v>67</v>
       </c>
-      <c r="R39" t="s">
+      <c r="R40" t="s">
         <v>114</v>
       </c>
-      <c r="S39" t="s">
+      <c r="S40" t="s">
         <v>110</v>
       </c>
-      <c r="T39">
+      <c r="T40">
         <f>1/1000000</f>
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>2022</v>
-      </c>
-      <c r="B40" t="s">
-        <v>115</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40">
-        <v>1000</v>
-      </c>
-      <c r="F40" t="s">
-        <v>123</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40" t="s">
-        <v>122</v>
-      </c>
-      <c r="I40">
-        <f t="shared" ref="I40:I43" si="3">-1000000</f>
-        <v>-1000000</v>
-      </c>
-      <c r="J40" t="s">
-        <v>70</v>
-      </c>
-      <c r="K40">
-        <v>1</v>
-      </c>
-      <c r="L40" t="s">
-        <v>125</v>
-      </c>
-      <c r="O40" t="s">
-        <v>115</v>
-      </c>
-      <c r="P40" t="s">
-        <v>67</v>
-      </c>
-      <c r="R40" t="s">
-        <v>115</v>
-      </c>
-      <c r="S40" t="s">
-        <v>110</v>
-      </c>
-      <c r="T40">
-        <f t="shared" ref="T40:T43" si="4">1/1000000</f>
-        <v>9.9999999999999995E-7</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2022</v>
       </c>
       <c r="B41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C41" s="6" t="s">
         <v>119</v>
@@ -6847,7 +6861,7 @@
         <v>122</v>
       </c>
       <c r="I41">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I41:I44" si="3">-1000000</f>
         <v>-1000000</v>
       </c>
       <c r="J41" t="s">
@@ -6860,28 +6874,28 @@
         <v>125</v>
       </c>
       <c r="O41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="P41" t="s">
         <v>67</v>
       </c>
       <c r="R41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S41" t="s">
         <v>110</v>
       </c>
       <c r="T41">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="T41:T44" si="4">1/1000000</f>
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2022</v>
       </c>
       <c r="B42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>119</v>
@@ -6915,13 +6929,13 @@
         <v>125</v>
       </c>
       <c r="O42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P42" t="s">
         <v>67</v>
       </c>
       <c r="R42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S42" t="s">
         <v>110</v>
@@ -6931,12 +6945,12 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2022</v>
       </c>
       <c r="B43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>119</v>
@@ -6970,13 +6984,13 @@
         <v>125</v>
       </c>
       <c r="O43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P43" t="s">
         <v>67</v>
       </c>
       <c r="R43" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S43" t="s">
         <v>110</v>
@@ -6986,84 +7000,88 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44">
+        <v>2022</v>
+      </c>
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" t="s">
+        <v>119</v>
+      </c>
+      <c r="E44">
+        <v>1000</v>
+      </c>
+      <c r="F44" t="s">
+        <v>123</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="s">
+        <v>122</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="3"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J44" t="s">
+        <v>70</v>
+      </c>
+      <c r="K44">
+        <v>1</v>
+      </c>
+      <c r="L44" t="s">
+        <v>125</v>
+      </c>
+      <c r="O44" t="s">
+        <v>118</v>
+      </c>
+      <c r="P44" t="s">
+        <v>67</v>
+      </c>
+      <c r="R44" t="s">
+        <v>118</v>
+      </c>
+      <c r="S44" t="s">
+        <v>110</v>
+      </c>
+      <c r="T44">
+        <f t="shared" si="4"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A45">
         <v>2033</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>128</v>
-      </c>
-      <c r="C44" t="s">
-        <v>127</v>
-      </c>
-      <c r="D44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44" t="s">
-        <v>66</v>
-      </c>
-      <c r="G44">
-        <v>601.34999999999991</v>
-      </c>
-      <c r="H44" t="s">
-        <v>81</v>
-      </c>
-      <c r="I44">
-        <v>-363</v>
-      </c>
-      <c r="J44" t="s">
-        <v>69</v>
-      </c>
-      <c r="K44">
-        <v>5</v>
-      </c>
-      <c r="O44" t="s">
-        <v>82</v>
-      </c>
-      <c r="P44" t="s">
-        <v>59</v>
-      </c>
-      <c r="R44" t="s">
-        <v>131</v>
-      </c>
-      <c r="S44" t="s">
-        <v>111</v>
-      </c>
-      <c r="T44">
-        <f>1/3.6/1000000</f>
-        <v>2.7777777777777781E-7</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>2022</v>
-      </c>
-      <c r="B45" t="s">
-        <v>129</v>
       </c>
       <c r="C45" t="s">
         <v>127</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="G45">
-        <v>3600</v>
+        <v>601.34999999999991</v>
       </c>
       <c r="H45" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="I45">
-        <v>80</v>
+        <v>-363</v>
       </c>
       <c r="J45" t="s">
         <v>69</v>
@@ -7088,12 +7106,12 @@
         <v>2.7777777777777781E-7</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2022</v>
       </c>
       <c r="B46" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C46" t="s">
         <v>127</v>
@@ -7102,7 +7120,7 @@
         <v>45</v>
       </c>
       <c r="E46">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F46" t="s">
         <v>62</v>
@@ -7114,7 +7132,7 @@
         <v>63</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J46" t="s">
         <v>69</v>
@@ -7141,37 +7159,37 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>2034</v>
+        <v>2022</v>
       </c>
       <c r="B47" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C47" t="s">
-        <v>29</v>
+        <v>127</v>
       </c>
       <c r="D47" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="E47">
-        <v>11.4</v>
+        <v>18</v>
       </c>
       <c r="F47" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G47">
-        <v>1055</v>
-      </c>
-      <c r="H47" s="12" t="s">
-        <v>81</v>
+        <v>3600</v>
+      </c>
+      <c r="H47" t="s">
+        <v>63</v>
       </c>
       <c r="I47">
-        <v>40</v>
-      </c>
-      <c r="J47" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J47" t="s">
         <v>69</v>
       </c>
       <c r="K47">
-        <v>0.9</v>
+        <v>5</v>
       </c>
       <c r="O47" t="s">
         <v>82</v>
@@ -7180,121 +7198,121 @@
         <v>59</v>
       </c>
       <c r="R47" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="S47" t="s">
+        <v>111</v>
+      </c>
+      <c r="T47">
+        <f>1/3.6/1000000</f>
+        <v>2.7777777777777781E-7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2034</v>
+      </c>
+      <c r="B48" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48">
+        <v>11.4</v>
+      </c>
+      <c r="F48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G48">
+        <v>1055</v>
+      </c>
+      <c r="H48" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I48">
+        <v>200</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="K48">
+        <v>0.9</v>
+      </c>
+      <c r="O48" t="s">
+        <v>82</v>
+      </c>
+      <c r="P48" t="s">
+        <v>59</v>
+      </c>
+      <c r="R48" t="s">
+        <v>139</v>
+      </c>
+      <c r="S48" t="s">
         <v>109</v>
       </c>
-      <c r="T47">
+      <c r="T48">
         <f>1/134.47/1000000</f>
         <v>7.436602959767978E-9</v>
       </c>
     </row>
-    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A49">
         <v>2034</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>92</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>46</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D49" t="s">
         <v>137</v>
       </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
         <v>66</v>
       </c>
-      <c r="G48">
+      <c r="G49">
         <v>601.34999999999991</v>
       </c>
-      <c r="H48" t="s">
+      <c r="H49" t="s">
         <v>81</v>
       </c>
-      <c r="I48">
-        <v>70</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="I49">
+        <v>150</v>
+      </c>
+      <c r="J49" t="s">
         <v>69</v>
       </c>
-      <c r="K48">
+      <c r="K49">
         <v>3.4</v>
       </c>
-      <c r="O48" t="s">
+      <c r="O49" t="s">
         <v>82</v>
       </c>
-      <c r="P48" t="s">
+      <c r="P49" t="s">
         <v>60</v>
       </c>
-      <c r="R48" t="s">
+      <c r="R49" t="s">
         <v>98</v>
       </c>
-      <c r="S48" t="s">
+      <c r="S49" t="s">
         <v>111</v>
       </c>
-      <c r="T48">
+      <c r="T49">
         <f>1/3.6/1000000</f>
         <v>2.7777777777777781E-7</v>
       </c>
     </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50">
         <v>2022</v>
-      </c>
-      <c r="B49" t="s">
-        <v>52</v>
-      </c>
-      <c r="C49" t="s">
-        <v>49</v>
-      </c>
-      <c r="D49" t="s">
-        <v>50</v>
-      </c>
-      <c r="E49">
-        <v>42</v>
-      </c>
-      <c r="F49" t="s">
-        <v>66</v>
-      </c>
-      <c r="G49">
-        <v>1055</v>
-      </c>
-      <c r="H49" t="s">
-        <v>81</v>
-      </c>
-      <c r="I49">
-        <v>116</v>
-      </c>
-      <c r="J49" t="s">
-        <v>69</v>
-      </c>
-      <c r="K49">
-        <v>1.9</v>
-      </c>
-      <c r="O49" t="s">
-        <v>82</v>
-      </c>
-      <c r="P49" t="s">
-        <v>59</v>
-      </c>
-      <c r="R49" t="s">
-        <v>99</v>
-      </c>
-      <c r="S49" t="s">
-        <v>108</v>
-      </c>
-      <c r="T49">
-        <f>1/120/1000000</f>
-        <v>8.3333333333333335E-9</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>2034</v>
       </c>
       <c r="B50" t="s">
         <v>52</v>
@@ -7303,22 +7321,22 @@
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
       <c r="E50">
-        <v>42.706773295182977</v>
+        <v>42</v>
       </c>
       <c r="F50" t="s">
         <v>66</v>
       </c>
       <c r="G50">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H50" t="s">
         <v>81</v>
       </c>
       <c r="I50">
-        <v>60</v>
+        <v>116</v>
       </c>
       <c r="J50" t="s">
         <v>69</v>
@@ -7343,48 +7361,48 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2034</v>
       </c>
       <c r="B51" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="C51" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="D51" t="s">
         <v>136</v>
       </c>
       <c r="E51">
-        <v>42.706773295182977</v>
+        <v>52.1</v>
       </c>
       <c r="F51" t="s">
         <v>66</v>
       </c>
       <c r="G51">
-        <v>1055</v>
+        <v>865.1</v>
       </c>
       <c r="H51" t="s">
         <v>81</v>
       </c>
       <c r="I51">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="J51" t="s">
         <v>69</v>
       </c>
       <c r="K51">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
       <c r="O51" t="s">
         <v>82</v>
       </c>
       <c r="P51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R51" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="S51" t="s">
         <v>108</v>
@@ -7394,117 +7412,117 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2034</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>90</v>
       </c>
       <c r="C52" t="s">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>52.1</v>
       </c>
       <c r="F52" t="s">
         <v>66</v>
       </c>
       <c r="G52">
-        <v>601.34999999999991</v>
-      </c>
-      <c r="H52" s="12" t="s">
+        <v>865.1</v>
+      </c>
+      <c r="H52" t="s">
         <v>81</v>
       </c>
       <c r="I52">
-        <v>70</v>
+        <v>200</v>
       </c>
       <c r="J52" t="s">
         <v>69</v>
       </c>
       <c r="K52">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="O52" t="s">
         <v>82</v>
       </c>
       <c r="P52" t="s">
+        <v>60</v>
+      </c>
+      <c r="R52" t="s">
+        <v>103</v>
+      </c>
+      <c r="S52" t="s">
+        <v>108</v>
+      </c>
+      <c r="T52">
+        <f>1/120/1000000</f>
+        <v>8.3333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2034</v>
+      </c>
+      <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
+        <v>127</v>
+      </c>
+      <c r="D53" t="s">
+        <v>137</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>66</v>
+      </c>
+      <c r="G53">
+        <v>601.34999999999991</v>
+      </c>
+      <c r="H53" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I53">
+        <v>150</v>
+      </c>
+      <c r="J53" t="s">
+        <v>69</v>
+      </c>
+      <c r="K53">
+        <v>5</v>
+      </c>
+      <c r="O53" t="s">
+        <v>82</v>
+      </c>
+      <c r="P53" t="s">
         <v>59</v>
       </c>
-      <c r="R52" t="s">
+      <c r="R53" t="s">
         <v>131</v>
       </c>
-      <c r="S52" t="s">
+      <c r="S53" t="s">
         <v>111</v>
       </c>
-      <c r="T52">
+      <c r="T53">
         <f>1/3.6/1000000</f>
         <v>2.7777777777777781E-7</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>2022</v>
-      </c>
-      <c r="B53" t="s">
-        <v>49</v>
-      </c>
-      <c r="C53" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" t="s">
-        <v>45</v>
-      </c>
-      <c r="E53">
-        <v>86</v>
-      </c>
-      <c r="F53" t="s">
-        <v>62</v>
-      </c>
-      <c r="G53">
-        <v>2066.4</v>
-      </c>
-      <c r="H53" t="s">
-        <v>63</v>
-      </c>
-      <c r="I53">
-        <v>164.46</v>
-      </c>
-      <c r="J53" t="s">
-        <v>69</v>
-      </c>
-      <c r="K53">
-        <v>1.9</v>
-      </c>
-      <c r="O53" t="s">
-        <v>82</v>
-      </c>
-      <c r="P53" t="s">
-        <v>59</v>
-      </c>
-      <c r="R53" t="s">
-        <v>99</v>
-      </c>
-      <c r="S53" t="s">
-        <v>108</v>
-      </c>
-      <c r="T53">
-        <f>1/120/1000000</f>
-        <v>8.3333333333333335E-9</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2022</v>
       </c>
       <c r="B54" t="s">
-        <v>89</v>
+        <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="D54" t="s">
         <v>45</v>
@@ -7518,7 +7536,7 @@
       <c r="G54">
         <v>2066.4</v>
       </c>
-      <c r="H54" s="12" t="s">
+      <c r="H54" t="s">
         <v>63</v>
       </c>
       <c r="I54">
@@ -7528,16 +7546,16 @@
         <v>69</v>
       </c>
       <c r="K54">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
       <c r="O54" t="s">
         <v>82</v>
       </c>
       <c r="P54" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R54" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="S54" t="s">
         <v>108</v>
@@ -7547,21 +7565,21 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2022</v>
       </c>
       <c r="B55" t="s">
-        <v>139</v>
+        <v>90</v>
       </c>
       <c r="C55" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="D55" t="s">
         <v>45</v>
       </c>
       <c r="E55">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="F55" t="s">
         <v>62</v>
@@ -7569,26 +7587,26 @@
       <c r="G55">
         <v>2066.4</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H55" s="12" t="s">
         <v>63</v>
       </c>
       <c r="I55">
-        <v>10.51</v>
+        <v>164.46</v>
       </c>
       <c r="J55" t="s">
         <v>69</v>
       </c>
       <c r="K55">
-        <v>1.9</v>
+        <v>2.5</v>
       </c>
       <c r="O55" t="s">
         <v>82</v>
       </c>
       <c r="P55" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R55" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="S55" t="s">
         <v>108</v>
@@ -7598,15 +7616,15 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2022</v>
       </c>
       <c r="B56" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C56" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="D56" t="s">
         <v>45</v>
@@ -7630,16 +7648,16 @@
         <v>69</v>
       </c>
       <c r="K56">
-        <v>2.5</v>
+        <v>1.9</v>
       </c>
       <c r="O56" t="s">
         <v>82</v>
       </c>
       <c r="P56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R56" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="S56" t="s">
         <v>108</v>
@@ -7649,16 +7667,890 @@
         <v>8.3333333333333335E-9</v>
       </c>
     </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>2022</v>
+      </c>
+      <c r="B57" t="s">
+        <v>143</v>
+      </c>
+      <c r="C57" t="s">
+        <v>89</v>
+      </c>
+      <c r="D57" t="s">
+        <v>45</v>
+      </c>
+      <c r="E57">
+        <v>137</v>
+      </c>
+      <c r="F57" t="s">
+        <v>62</v>
+      </c>
+      <c r="G57">
+        <v>2066.4</v>
+      </c>
+      <c r="H57" t="s">
+        <v>63</v>
+      </c>
+      <c r="I57">
+        <v>10.51</v>
+      </c>
+      <c r="J57" t="s">
+        <v>69</v>
+      </c>
+      <c r="K57">
+        <v>2.5</v>
+      </c>
+      <c r="O57" t="s">
+        <v>82</v>
+      </c>
+      <c r="P57" t="s">
+        <v>60</v>
+      </c>
+      <c r="R57" t="s">
+        <v>103</v>
+      </c>
+      <c r="S57" t="s">
+        <v>108</v>
+      </c>
+      <c r="T57">
+        <f>1/120/1000000</f>
+        <v>8.3333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>2030</v>
+      </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
+      <c r="C58" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" t="s">
+        <v>48</v>
+      </c>
+      <c r="E58" s="21">
+        <v>1000</v>
+      </c>
+      <c r="F58" t="s">
+        <v>56</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58" t="s">
+        <v>57</v>
+      </c>
+      <c r="I58">
+        <f>-1000000</f>
+        <v>-1000000</v>
+      </c>
+      <c r="J58" t="s">
+        <v>70</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="O58" t="s">
+        <v>82</v>
+      </c>
+      <c r="P58" t="s">
+        <v>67</v>
+      </c>
+      <c r="R58" t="s">
+        <v>102</v>
+      </c>
+      <c r="S58" t="s">
+        <v>110</v>
+      </c>
+      <c r="T58">
+        <f>1/1000000</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>2031</v>
+      </c>
+      <c r="B59" t="s">
+        <v>55</v>
+      </c>
+      <c r="C59" t="s">
+        <v>55</v>
+      </c>
+      <c r="D59" t="s">
+        <v>48</v>
+      </c>
+      <c r="E59" s="21">
+        <v>908</v>
+      </c>
+      <c r="F59" t="s">
+        <v>56</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59" t="s">
+        <v>57</v>
+      </c>
+      <c r="I59">
+        <f t="shared" ref="I59:I73" si="5">-1000000</f>
+        <v>-1000000</v>
+      </c>
+      <c r="J59" t="s">
+        <v>70</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="O59" t="s">
+        <v>82</v>
+      </c>
+      <c r="P59" t="s">
+        <v>67</v>
+      </c>
+      <c r="R59" t="s">
+        <v>102</v>
+      </c>
+      <c r="S59" t="s">
+        <v>110</v>
+      </c>
+      <c r="T59">
+        <f t="shared" ref="T59:T73" si="6">1/1000000</f>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>2032</v>
+      </c>
+      <c r="B60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C60" t="s">
+        <v>55</v>
+      </c>
+      <c r="D60" t="s">
+        <v>48</v>
+      </c>
+      <c r="E60" s="21">
+        <v>825</v>
+      </c>
+      <c r="F60" t="s">
+        <v>56</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" t="s">
+        <v>57</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J60" t="s">
+        <v>70</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="O60" t="s">
+        <v>82</v>
+      </c>
+      <c r="P60" t="s">
+        <v>67</v>
+      </c>
+      <c r="R60" t="s">
+        <v>102</v>
+      </c>
+      <c r="S60" t="s">
+        <v>110</v>
+      </c>
+      <c r="T60">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>2033</v>
+      </c>
+      <c r="B61" t="s">
+        <v>55</v>
+      </c>
+      <c r="C61" t="s">
+        <v>55</v>
+      </c>
+      <c r="D61" t="s">
+        <v>48</v>
+      </c>
+      <c r="E61" s="21">
+        <v>749</v>
+      </c>
+      <c r="F61" t="s">
+        <v>56</v>
+      </c>
+      <c r="G61">
+        <v>1</v>
+      </c>
+      <c r="H61" t="s">
+        <v>57</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J61" t="s">
+        <v>70</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+      <c r="O61" t="s">
+        <v>82</v>
+      </c>
+      <c r="P61" t="s">
+        <v>67</v>
+      </c>
+      <c r="R61" t="s">
+        <v>102</v>
+      </c>
+      <c r="S61" t="s">
+        <v>110</v>
+      </c>
+      <c r="T61">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2034</v>
+      </c>
+      <c r="B62" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" t="s">
+        <v>55</v>
+      </c>
+      <c r="D62" t="s">
+        <v>48</v>
+      </c>
+      <c r="E62" s="21">
+        <v>680</v>
+      </c>
+      <c r="F62" t="s">
+        <v>56</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="H62" t="s">
+        <v>57</v>
+      </c>
+      <c r="I62">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J62" t="s">
+        <v>70</v>
+      </c>
+      <c r="K62">
+        <v>1</v>
+      </c>
+      <c r="O62" t="s">
+        <v>82</v>
+      </c>
+      <c r="P62" t="s">
+        <v>67</v>
+      </c>
+      <c r="R62" t="s">
+        <v>102</v>
+      </c>
+      <c r="S62" t="s">
+        <v>110</v>
+      </c>
+      <c r="T62">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>2035</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>55</v>
+      </c>
+      <c r="D63" t="s">
+        <v>48</v>
+      </c>
+      <c r="E63" s="21">
+        <v>618</v>
+      </c>
+      <c r="F63" t="s">
+        <v>56</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63" t="s">
+        <v>57</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J63" t="s">
+        <v>70</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="O63" t="s">
+        <v>82</v>
+      </c>
+      <c r="P63" t="s">
+        <v>67</v>
+      </c>
+      <c r="R63" t="s">
+        <v>102</v>
+      </c>
+      <c r="S63" t="s">
+        <v>110</v>
+      </c>
+      <c r="T63">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>2036</v>
+      </c>
+      <c r="B64" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" t="s">
+        <v>55</v>
+      </c>
+      <c r="D64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E64" s="21">
+        <v>561</v>
+      </c>
+      <c r="F64" t="s">
+        <v>56</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" t="s">
+        <v>57</v>
+      </c>
+      <c r="I64">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J64" t="s">
+        <v>70</v>
+      </c>
+      <c r="K64">
+        <v>1</v>
+      </c>
+      <c r="O64" t="s">
+        <v>82</v>
+      </c>
+      <c r="P64" t="s">
+        <v>67</v>
+      </c>
+      <c r="R64" t="s">
+        <v>102</v>
+      </c>
+      <c r="S64" t="s">
+        <v>110</v>
+      </c>
+      <c r="T64">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>2037</v>
+      </c>
+      <c r="B65" t="s">
+        <v>55</v>
+      </c>
+      <c r="C65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D65" t="s">
+        <v>48</v>
+      </c>
+      <c r="E65" s="21">
+        <v>510</v>
+      </c>
+      <c r="F65" t="s">
+        <v>56</v>
+      </c>
+      <c r="G65">
+        <v>1</v>
+      </c>
+      <c r="H65" t="s">
+        <v>57</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J65" t="s">
+        <v>70</v>
+      </c>
+      <c r="K65">
+        <v>1</v>
+      </c>
+      <c r="O65" t="s">
+        <v>82</v>
+      </c>
+      <c r="P65" t="s">
+        <v>67</v>
+      </c>
+      <c r="R65" t="s">
+        <v>102</v>
+      </c>
+      <c r="S65" t="s">
+        <v>110</v>
+      </c>
+      <c r="T65">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>2038</v>
+      </c>
+      <c r="B66" t="s">
+        <v>55</v>
+      </c>
+      <c r="C66" t="s">
+        <v>55</v>
+      </c>
+      <c r="D66" t="s">
+        <v>48</v>
+      </c>
+      <c r="E66" s="21">
+        <v>463</v>
+      </c>
+      <c r="F66" t="s">
+        <v>56</v>
+      </c>
+      <c r="G66">
+        <v>1</v>
+      </c>
+      <c r="H66" t="s">
+        <v>57</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J66" t="s">
+        <v>70</v>
+      </c>
+      <c r="K66">
+        <v>1</v>
+      </c>
+      <c r="O66" t="s">
+        <v>82</v>
+      </c>
+      <c r="P66" t="s">
+        <v>67</v>
+      </c>
+      <c r="R66" t="s">
+        <v>102</v>
+      </c>
+      <c r="S66" t="s">
+        <v>110</v>
+      </c>
+      <c r="T66">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>2039</v>
+      </c>
+      <c r="B67" t="s">
+        <v>55</v>
+      </c>
+      <c r="C67" t="s">
+        <v>55</v>
+      </c>
+      <c r="D67" t="s">
+        <v>48</v>
+      </c>
+      <c r="E67" s="21">
+        <v>420</v>
+      </c>
+      <c r="F67" t="s">
+        <v>56</v>
+      </c>
+      <c r="G67">
+        <v>1</v>
+      </c>
+      <c r="H67" t="s">
+        <v>57</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J67" t="s">
+        <v>70</v>
+      </c>
+      <c r="K67">
+        <v>1</v>
+      </c>
+      <c r="O67" t="s">
+        <v>82</v>
+      </c>
+      <c r="P67" t="s">
+        <v>67</v>
+      </c>
+      <c r="R67" t="s">
+        <v>102</v>
+      </c>
+      <c r="S67" t="s">
+        <v>110</v>
+      </c>
+      <c r="T67">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>2040</v>
+      </c>
+      <c r="B68" t="s">
+        <v>55</v>
+      </c>
+      <c r="C68" t="s">
+        <v>55</v>
+      </c>
+      <c r="D68" t="s">
+        <v>48</v>
+      </c>
+      <c r="E68" s="21">
+        <v>382</v>
+      </c>
+      <c r="F68" t="s">
+        <v>56</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68" t="s">
+        <v>57</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J68" t="s">
+        <v>70</v>
+      </c>
+      <c r="K68">
+        <v>1</v>
+      </c>
+      <c r="O68" t="s">
+        <v>82</v>
+      </c>
+      <c r="P68" t="s">
+        <v>67</v>
+      </c>
+      <c r="R68" t="s">
+        <v>102</v>
+      </c>
+      <c r="S68" t="s">
+        <v>110</v>
+      </c>
+      <c r="T68">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>2041</v>
+      </c>
+      <c r="B69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C69" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" t="s">
+        <v>48</v>
+      </c>
+      <c r="E69" s="21">
+        <v>347</v>
+      </c>
+      <c r="F69" t="s">
+        <v>56</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69" t="s">
+        <v>57</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J69" t="s">
+        <v>70</v>
+      </c>
+      <c r="K69">
+        <v>1</v>
+      </c>
+      <c r="O69" t="s">
+        <v>82</v>
+      </c>
+      <c r="P69" t="s">
+        <v>67</v>
+      </c>
+      <c r="R69" t="s">
+        <v>102</v>
+      </c>
+      <c r="S69" t="s">
+        <v>110</v>
+      </c>
+      <c r="T69">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>2042</v>
+      </c>
+      <c r="B70" t="s">
+        <v>55</v>
+      </c>
+      <c r="C70" t="s">
+        <v>55</v>
+      </c>
+      <c r="D70" t="s">
+        <v>48</v>
+      </c>
+      <c r="E70" s="21">
+        <v>315</v>
+      </c>
+      <c r="F70" t="s">
+        <v>56</v>
+      </c>
+      <c r="G70">
+        <v>1</v>
+      </c>
+      <c r="H70" t="s">
+        <v>57</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J70" t="s">
+        <v>70</v>
+      </c>
+      <c r="K70">
+        <v>1</v>
+      </c>
+      <c r="O70" t="s">
+        <v>82</v>
+      </c>
+      <c r="P70" t="s">
+        <v>67</v>
+      </c>
+      <c r="R70" t="s">
+        <v>102</v>
+      </c>
+      <c r="S70" t="s">
+        <v>110</v>
+      </c>
+      <c r="T70">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>2043</v>
+      </c>
+      <c r="B71" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" t="s">
+        <v>48</v>
+      </c>
+      <c r="E71" s="21">
+        <v>286</v>
+      </c>
+      <c r="F71" t="s">
+        <v>56</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71" t="s">
+        <v>57</v>
+      </c>
+      <c r="I71">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J71" t="s">
+        <v>70</v>
+      </c>
+      <c r="K71">
+        <v>1</v>
+      </c>
+      <c r="O71" t="s">
+        <v>82</v>
+      </c>
+      <c r="P71" t="s">
+        <v>67</v>
+      </c>
+      <c r="R71" t="s">
+        <v>102</v>
+      </c>
+      <c r="S71" t="s">
+        <v>110</v>
+      </c>
+      <c r="T71">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>2044</v>
+      </c>
+      <c r="B72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C72" t="s">
+        <v>55</v>
+      </c>
+      <c r="D72" t="s">
+        <v>48</v>
+      </c>
+      <c r="E72" s="21">
+        <v>260</v>
+      </c>
+      <c r="F72" t="s">
+        <v>56</v>
+      </c>
+      <c r="G72">
+        <v>1</v>
+      </c>
+      <c r="H72" t="s">
+        <v>57</v>
+      </c>
+      <c r="I72">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J72" t="s">
+        <v>70</v>
+      </c>
+      <c r="K72">
+        <v>1</v>
+      </c>
+      <c r="O72" t="s">
+        <v>82</v>
+      </c>
+      <c r="P72" t="s">
+        <v>67</v>
+      </c>
+      <c r="R72" t="s">
+        <v>102</v>
+      </c>
+      <c r="S72" t="s">
+        <v>110</v>
+      </c>
+      <c r="T72">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>2045</v>
+      </c>
+      <c r="B73" t="s">
+        <v>55</v>
+      </c>
+      <c r="C73" t="s">
+        <v>55</v>
+      </c>
+      <c r="D73" t="s">
+        <v>48</v>
+      </c>
+      <c r="E73" s="21">
+        <v>236</v>
+      </c>
+      <c r="F73" t="s">
+        <v>56</v>
+      </c>
+      <c r="G73">
+        <v>1</v>
+      </c>
+      <c r="H73" t="s">
+        <v>57</v>
+      </c>
+      <c r="I73">
+        <f t="shared" si="5"/>
+        <v>-1000000</v>
+      </c>
+      <c r="J73" t="s">
+        <v>70</v>
+      </c>
+      <c r="K73">
+        <v>1</v>
+      </c>
+      <c r="O73" t="s">
+        <v>82</v>
+      </c>
+      <c r="P73" t="s">
+        <v>67</v>
+      </c>
+      <c r="R73" t="s">
+        <v>102</v>
+      </c>
+      <c r="S73" t="s">
+        <v>110</v>
+      </c>
+      <c r="T73">
+        <f t="shared" si="6"/>
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:U56" xr:uid="{07BB7D1A-D496-4ED1-ADCB-0A74F600D4AC}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="CNG"/>
-        <filter val="CNG from Dairies"/>
-        <filter val="Landfill CNG"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7731,10 +8623,10 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:D124"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="D126" sqref="D126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9145,7 +10037,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>2040</v>
@@ -9159,7 +10051,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>2040</v>
@@ -9173,7 +10065,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>2041</v>
@@ -9187,7 +10079,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>2041</v>
@@ -9201,7 +10093,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>2042</v>
@@ -9215,7 +10107,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>2042</v>
@@ -9229,7 +10121,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>2043</v>
@@ -9243,7 +10135,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>2043</v>
@@ -9257,7 +10149,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>2044</v>
@@ -9271,7 +10163,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>2044</v>
@@ -9285,7 +10177,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>2045</v>
@@ -9299,7 +10191,7 @@
         <v>inf</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>2045</v>
@@ -9311,6 +10203,21 @@
       <c r="C124" t="str">
         <f t="shared" si="46"/>
         <v>inf</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>2022</v>
+      </c>
+      <c r="B125" t="s">
+        <v>38</v>
+      </c>
+      <c r="C125">
+        <f>300*1000000*129</f>
+        <v>38700000000</v>
+      </c>
+      <c r="D125">
+        <v>0.4</v>
       </c>
     </row>
   </sheetData>
@@ -9323,8 +10230,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:BV14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AM3" sqref="AM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9531,9 +10438,6 @@
         <f>AK2</f>
         <v>361325</v>
       </c>
-      <c r="AM2" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="3" spans="1:74" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -9565,6 +10469,9 @@
       </c>
       <c r="AL3">
         <v>309035</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>71</v>
       </c>
       <c r="AN3" s="9"/>
       <c r="AO3" s="9"/>

</xml_diff>